<commit_message>
matrix prediction with CNN and LSTM
</commit_message>
<xml_diff>
--- a/portfolio-optimization/optimization.xlsx
+++ b/portfolio-optimization/optimization.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Desktop\Projects\VAR_COV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Desktop\Projects\Spring-2025-Internship-Resources\portfolio-optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F4C262-CA2D-4A35-9EC1-84B1463112A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553ABA79-4CBE-45D9-B080-67F510894649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -904,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>